<commit_message>
current with Major 4
</commit_message>
<xml_diff>
--- a/v04/data/vetoes.xlsx
+++ b/v04/data/vetoes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a37d342720a2caaa/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a37d342720a2caaa/Desktop/dataClass/06-cod-analysis/03 CDL PrizePicks Betting/cdl_prizepicks_betting_apps/v04/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2282" documentId="11_05A95047836714DFE54878D6425DCE3A87460B4D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E15F0F0A-4612-4DFC-9D1B-1858D4F4CEE8}"/>
+  <xr:revisionPtr revIDLastSave="2341" documentId="11_05A95047836714DFE54878D6425DCE3A87460B4D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EC71C7C-D82B-4122-83CE-61355F67A309}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2170" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2206" uniqueCount="32">
   <si>
     <t>match_id</t>
   </si>
@@ -219,10 +219,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -510,10 +506,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J361"/>
+  <dimension ref="A1:J367"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <pane ySplit="1" topLeftCell="A347" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O366" sqref="O366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -10997,6 +10994,180 @@
         <v>30</v>
       </c>
     </row>
+    <row r="362" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A362" s="5">
+        <v>27319</v>
+      </c>
+      <c r="B362" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C362" s="7">
+        <v>4</v>
+      </c>
+      <c r="D362" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E362" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F362" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G362" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H362" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J362" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="363" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A363" s="5">
+        <v>27319</v>
+      </c>
+      <c r="B363" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C363" s="7">
+        <v>4</v>
+      </c>
+      <c r="D363" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E363" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F363" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G363" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H363" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I363" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="364" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A364" s="5">
+        <v>27320</v>
+      </c>
+      <c r="B364" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C364" s="7">
+        <v>4</v>
+      </c>
+      <c r="D364" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E364" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F364" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G364" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H364" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I364" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="365" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A365" s="5">
+        <v>27320</v>
+      </c>
+      <c r="B365" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C365" s="7">
+        <v>4</v>
+      </c>
+      <c r="D365" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E365" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F365" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G365" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H365" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J365" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="366" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A366" s="5">
+        <v>27321</v>
+      </c>
+      <c r="B366" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C366" s="7">
+        <v>4</v>
+      </c>
+      <c r="D366" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E366" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F366" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G366" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H366" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J366" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="367" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A367" s="5">
+        <v>27321</v>
+      </c>
+      <c r="B367" s="4">
+        <v>45443</v>
+      </c>
+      <c r="C367" s="7">
+        <v>4</v>
+      </c>
+      <c r="D367" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E367" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F367" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G367" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H367" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I367" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updated match info and streak icons.
</commit_message>
<xml_diff>
--- a/v04/data/vetoes.xlsx
+++ b/v04/data/vetoes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a37d342720a2caaa/Desktop/dataClass/06-cod-analysis/03 CDL PrizePicks Betting/cdl_prizepicks_betting_apps/v04/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2341" documentId="11_05A95047836714DFE54878D6425DCE3A87460B4D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EC71C7C-D82B-4122-83CE-61355F67A309}"/>
+  <xr:revisionPtr revIDLastSave="2550" documentId="11_05A95047836714DFE54878D6425DCE3A87460B4D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F98CE7EF-5AF3-48A5-8A23-516F56413302}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2206" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2338" uniqueCount="32">
   <si>
     <t>match_id</t>
   </si>
@@ -219,6 +219,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -506,11 +510,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J367"/>
+  <dimension ref="A1:J389"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A347" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O366" sqref="O366"/>
+      <pane ySplit="1" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L392" sqref="L392"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -11168,6 +11172,644 @@
         <v>24</v>
       </c>
     </row>
+    <row r="368" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A368" s="5">
+        <v>27322</v>
+      </c>
+      <c r="B368" s="4">
+        <v>45444</v>
+      </c>
+      <c r="C368" s="7">
+        <v>4</v>
+      </c>
+      <c r="D368" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E368" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F368" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G368" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H368" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I368" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="369" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A369" s="5">
+        <v>27322</v>
+      </c>
+      <c r="B369" s="4">
+        <v>45444</v>
+      </c>
+      <c r="C369" s="7">
+        <v>4</v>
+      </c>
+      <c r="D369" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E369" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F369" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G369" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H369" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J369" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="370" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A370" s="5">
+        <v>27323</v>
+      </c>
+      <c r="B370" s="4">
+        <v>45444</v>
+      </c>
+      <c r="C370" s="7">
+        <v>4</v>
+      </c>
+      <c r="D370" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E370" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F370" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G370" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H370" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J370" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="371" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A371" s="5">
+        <v>27323</v>
+      </c>
+      <c r="B371" s="4">
+        <v>45444</v>
+      </c>
+      <c r="C371" s="7">
+        <v>4</v>
+      </c>
+      <c r="D371" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E371" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F371" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G371" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H371" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I371" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="372" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A372" s="5">
+        <v>27324</v>
+      </c>
+      <c r="B372" s="4">
+        <v>45444</v>
+      </c>
+      <c r="C372" s="7">
+        <v>4</v>
+      </c>
+      <c r="D372" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E372" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F372" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G372" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H372" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J372" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="373" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A373" s="5">
+        <v>27324</v>
+      </c>
+      <c r="B373" s="4">
+        <v>45444</v>
+      </c>
+      <c r="C373" s="7">
+        <v>4</v>
+      </c>
+      <c r="D373" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E373" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F373" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G373" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H373" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I373" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="374" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A374" s="5">
+        <v>27325</v>
+      </c>
+      <c r="B374" s="4">
+        <v>45444</v>
+      </c>
+      <c r="C374" s="7">
+        <v>4</v>
+      </c>
+      <c r="D374" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E374" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F374" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G374" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H374" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J374" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="375" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A375" s="5">
+        <v>27325</v>
+      </c>
+      <c r="B375" s="4">
+        <v>45444</v>
+      </c>
+      <c r="C375" s="7">
+        <v>4</v>
+      </c>
+      <c r="D375" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E375" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F375" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G375" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H375" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I375" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="376" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A376" s="5">
+        <v>27326</v>
+      </c>
+      <c r="B376" s="4">
+        <v>45445</v>
+      </c>
+      <c r="C376" s="7">
+        <v>4</v>
+      </c>
+      <c r="D376" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E376" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F376" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G376" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H376" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J376" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="377" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A377" s="5">
+        <v>27326</v>
+      </c>
+      <c r="B377" s="4">
+        <v>45445</v>
+      </c>
+      <c r="C377" s="7">
+        <v>4</v>
+      </c>
+      <c r="D377" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E377" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F377" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G377" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H377" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I377" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="378" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A378" s="5">
+        <v>27327</v>
+      </c>
+      <c r="B378" s="4">
+        <v>45445</v>
+      </c>
+      <c r="C378" s="7">
+        <v>4</v>
+      </c>
+      <c r="D378" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E378" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F378" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G378" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H378" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I378" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="379" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A379" s="5">
+        <v>27327</v>
+      </c>
+      <c r="B379" s="4">
+        <v>45445</v>
+      </c>
+      <c r="C379" s="7">
+        <v>4</v>
+      </c>
+      <c r="D379" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E379" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F379" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G379" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H379" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J379" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="380" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A380" s="5">
+        <v>27328</v>
+      </c>
+      <c r="B380" s="4">
+        <v>45445</v>
+      </c>
+      <c r="C380" s="7">
+        <v>4</v>
+      </c>
+      <c r="D380" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E380" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F380" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G380" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H380" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I380" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="381" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A381" s="5">
+        <v>27328</v>
+      </c>
+      <c r="B381" s="4">
+        <v>45445</v>
+      </c>
+      <c r="C381" s="7">
+        <v>4</v>
+      </c>
+      <c r="D381" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E381" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F381" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G381" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H381" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J381" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="382" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A382" s="5">
+        <v>27329</v>
+      </c>
+      <c r="B382" s="4">
+        <v>45445</v>
+      </c>
+      <c r="C382" s="7">
+        <v>4</v>
+      </c>
+      <c r="D382" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E382" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F382" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G382" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H382" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J382" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="383" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A383" s="5">
+        <v>27329</v>
+      </c>
+      <c r="B383" s="4">
+        <v>45445</v>
+      </c>
+      <c r="C383" s="7">
+        <v>4</v>
+      </c>
+      <c r="D383" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E383" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F383" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G383" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H383" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I383" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="384" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A384" s="5">
+        <v>27330</v>
+      </c>
+      <c r="B384" s="4">
+        <v>45450</v>
+      </c>
+      <c r="C384" s="7">
+        <v>4</v>
+      </c>
+      <c r="D384" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E384" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F384" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G384" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H384" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I384" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="385" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A385" s="5">
+        <v>27330</v>
+      </c>
+      <c r="B385" s="4">
+        <v>45450</v>
+      </c>
+      <c r="C385" s="7">
+        <v>4</v>
+      </c>
+      <c r="D385" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E385" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F385" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G385" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H385" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J385" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="386" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A386" s="5">
+        <v>27331</v>
+      </c>
+      <c r="B386" s="4">
+        <v>45450</v>
+      </c>
+      <c r="C386" s="7">
+        <v>4</v>
+      </c>
+      <c r="D386" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E386" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F386" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G386" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H386" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I386" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="387" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A387" s="5">
+        <v>27331</v>
+      </c>
+      <c r="B387" s="4">
+        <v>45450</v>
+      </c>
+      <c r="C387" s="7">
+        <v>4</v>
+      </c>
+      <c r="D387" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E387" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F387" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G387" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H387" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J387" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="388" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A388" s="5">
+        <v>27332</v>
+      </c>
+      <c r="B388" s="4">
+        <v>45450</v>
+      </c>
+      <c r="C388" s="7">
+        <v>4</v>
+      </c>
+      <c r="D388" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E388" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F388" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G388" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H388" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I388" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="389" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A389" s="5">
+        <v>27332</v>
+      </c>
+      <c r="B389" s="4">
+        <v>45450</v>
+      </c>
+      <c r="C389" s="7">
+        <v>4</v>
+      </c>
+      <c r="D389" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E389" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F389" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G389" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H389" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J389" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
finally fixed webscraper, works every time!
</commit_message>
<xml_diff>
--- a/v04/data/vetoes.xlsx
+++ b/v04/data/vetoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a37d342720a2caaa/Desktop/dataClass/06-cod-analysis/03 CDL PrizePicks Betting/cdl_prizepicks_betting_apps/v04/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2692" documentId="11_05A95047836714DFE54878D6425DCE3A87460B4D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC922246-CD97-415E-B0F3-798AFFA29296}"/>
+  <xr:revisionPtr revIDLastSave="2743" documentId="11_05A95047836714DFE54878D6425DCE3A87460B4D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{515F5E65-961C-401A-9830-CC65D127543E}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2422" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2458" uniqueCount="32">
   <si>
     <t>match_id</t>
   </si>
@@ -219,6 +219,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -506,11 +510,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J403"/>
+  <dimension ref="A1:J409"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A381" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U403" sqref="U403"/>
+      <pane ySplit="1" topLeftCell="A396" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F413" sqref="F413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -12212,6 +12216,180 @@
         <v>21</v>
       </c>
     </row>
+    <row r="404" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A404" s="5">
+        <v>27340</v>
+      </c>
+      <c r="B404" s="4">
+        <v>45457</v>
+      </c>
+      <c r="C404" s="7">
+        <v>4</v>
+      </c>
+      <c r="D404" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E404" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F404" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G404" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H404" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I404" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="405" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A405" s="5">
+        <v>27340</v>
+      </c>
+      <c r="B405" s="4">
+        <v>45457</v>
+      </c>
+      <c r="C405" s="7">
+        <v>4</v>
+      </c>
+      <c r="D405" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E405" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F405" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G405" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H405" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J405" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="406" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A406" s="5">
+        <v>27341</v>
+      </c>
+      <c r="B406" s="4">
+        <v>45457</v>
+      </c>
+      <c r="C406" s="7">
+        <v>4</v>
+      </c>
+      <c r="D406" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E406" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F406" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G406" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H406" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I406" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="407" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A407" s="5">
+        <v>27341</v>
+      </c>
+      <c r="B407" s="4">
+        <v>45457</v>
+      </c>
+      <c r="C407" s="7">
+        <v>4</v>
+      </c>
+      <c r="D407" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E407" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F407" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G407" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H407" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J407" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="408" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A408" s="5">
+        <v>27342</v>
+      </c>
+      <c r="B408" s="4">
+        <v>45457</v>
+      </c>
+      <c r="C408" s="7">
+        <v>4</v>
+      </c>
+      <c r="D408" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E408" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F408" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G408" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H408" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I408" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="409" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A409" s="5">
+        <v>27342</v>
+      </c>
+      <c r="B409" s="4">
+        <v>45457</v>
+      </c>
+      <c r="C409" s="7">
+        <v>4</v>
+      </c>
+      <c r="D409" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E409" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F409" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G409" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H409" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J409" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updated vetoes and added "by SnD Map" option to Page 2!
</commit_message>
<xml_diff>
--- a/v04/data/vetoes.xlsx
+++ b/v04/data/vetoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a37d342720a2caaa/Desktop/dataClass/06-cod-analysis/03 CDL PrizePicks Betting/cdl_prizepicks_betting_apps/v04/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2936" documentId="11_05A95047836714DFE54878D6425DCE3A87460B4D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1A92853-CE47-44AD-876C-A5D1D11D7A57}"/>
+  <xr:revisionPtr revIDLastSave="3289" documentId="11_05A95047836714DFE54878D6425DCE3A87460B4D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E6D0AD2-C40C-403F-BEF4-2DD827C506D3}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2590" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2842" uniqueCount="32">
   <si>
     <t>match_id</t>
   </si>
@@ -510,11 +510,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J431"/>
+  <dimension ref="A1:J473"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A410" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M428" sqref="M428"/>
+      <pane ySplit="1" topLeftCell="A455" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K471" sqref="K471"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -13028,6 +13028,1242 @@
         <v>21</v>
       </c>
     </row>
+    <row r="432" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A432" s="5">
+        <v>27354</v>
+      </c>
+      <c r="B432" s="4">
+        <v>45465</v>
+      </c>
+      <c r="C432" s="7">
+        <v>4</v>
+      </c>
+      <c r="D432" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E432" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F432" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G432" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H432" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I432" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="433" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A433" s="5">
+        <v>27354</v>
+      </c>
+      <c r="B433" s="4">
+        <v>45465</v>
+      </c>
+      <c r="C433" s="7">
+        <v>4</v>
+      </c>
+      <c r="D433" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E433" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F433" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G433" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H433" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J433" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="434" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A434" s="5">
+        <v>27355</v>
+      </c>
+      <c r="B434" s="4">
+        <v>45465</v>
+      </c>
+      <c r="C434" s="7">
+        <v>4</v>
+      </c>
+      <c r="D434" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E434" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F434" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G434" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H434" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I434" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="435" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A435" s="5">
+        <v>27355</v>
+      </c>
+      <c r="B435" s="4">
+        <v>45465</v>
+      </c>
+      <c r="C435" s="7">
+        <v>4</v>
+      </c>
+      <c r="D435" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E435" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F435" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G435" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H435" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J435" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="436" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A436" s="5">
+        <v>27356</v>
+      </c>
+      <c r="B436" s="4">
+        <v>45465</v>
+      </c>
+      <c r="C436" s="7">
+        <v>4</v>
+      </c>
+      <c r="D436" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E436" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F436" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G436" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H436" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I436" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="437" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A437" s="5">
+        <v>27356</v>
+      </c>
+      <c r="B437" s="4">
+        <v>45465</v>
+      </c>
+      <c r="C437" s="7">
+        <v>4</v>
+      </c>
+      <c r="D437" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E437" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F437" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G437" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H437" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J437" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="438" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A438" s="5">
+        <v>27357</v>
+      </c>
+      <c r="B438" s="4">
+        <v>45465</v>
+      </c>
+      <c r="C438" s="7">
+        <v>4</v>
+      </c>
+      <c r="D438" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E438" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F438" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G438" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H438" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I438" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="439" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A439" s="5">
+        <v>27357</v>
+      </c>
+      <c r="B439" s="4">
+        <v>45465</v>
+      </c>
+      <c r="C439" s="7">
+        <v>4</v>
+      </c>
+      <c r="D439" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E439" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F439" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G439" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H439" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J439" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="440" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A440" s="5">
+        <v>27358</v>
+      </c>
+      <c r="B440" s="4">
+        <v>45466</v>
+      </c>
+      <c r="C440" s="7">
+        <v>4</v>
+      </c>
+      <c r="D440" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E440" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F440" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G440" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H440" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I440" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="441" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A441" s="5">
+        <v>27358</v>
+      </c>
+      <c r="B441" s="4">
+        <v>45466</v>
+      </c>
+      <c r="C441" s="7">
+        <v>4</v>
+      </c>
+      <c r="D441" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E441" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F441" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G441" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H441" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J441" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="442" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A442" s="5">
+        <v>27359</v>
+      </c>
+      <c r="B442" s="4">
+        <v>45466</v>
+      </c>
+      <c r="C442" s="7">
+        <v>4</v>
+      </c>
+      <c r="D442" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E442" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F442" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G442" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H442" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I442" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="443" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A443" s="5">
+        <v>27359</v>
+      </c>
+      <c r="B443" s="4">
+        <v>45466</v>
+      </c>
+      <c r="C443" s="7">
+        <v>4</v>
+      </c>
+      <c r="D443" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E443" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F443" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G443" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H443" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J443" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="444" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A444" s="5">
+        <v>27360</v>
+      </c>
+      <c r="B444" s="4">
+        <v>45466</v>
+      </c>
+      <c r="C444" s="7">
+        <v>4</v>
+      </c>
+      <c r="D444" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E444" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F444" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G444" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H444" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I444" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="445" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A445" s="5">
+        <v>27360</v>
+      </c>
+      <c r="B445" s="4">
+        <v>45466</v>
+      </c>
+      <c r="C445" s="7">
+        <v>4</v>
+      </c>
+      <c r="D445" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E445" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F445" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G445" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H445" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J445" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="446" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A446" s="5">
+        <v>91336</v>
+      </c>
+      <c r="B446" s="4">
+        <v>45470</v>
+      </c>
+      <c r="C446" s="7">
+        <v>4</v>
+      </c>
+      <c r="D446" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E446" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F446" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G446" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H446" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I446" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="447" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A447" s="5">
+        <v>91336</v>
+      </c>
+      <c r="B447" s="4">
+        <v>45470</v>
+      </c>
+      <c r="C447" s="7">
+        <v>4</v>
+      </c>
+      <c r="D447" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E447" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F447" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G447" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H447" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J447" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="448" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A448" s="5">
+        <v>91337</v>
+      </c>
+      <c r="B448" s="4">
+        <v>45470</v>
+      </c>
+      <c r="C448" s="7">
+        <v>4</v>
+      </c>
+      <c r="D448" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E448" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F448" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G448" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H448" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I448" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="449" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A449" s="5">
+        <v>91337</v>
+      </c>
+      <c r="B449" s="4">
+        <v>45470</v>
+      </c>
+      <c r="C449" s="7">
+        <v>4</v>
+      </c>
+      <c r="D449" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E449" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F449" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G449" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H449" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J449" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="450" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A450" s="5">
+        <v>91338</v>
+      </c>
+      <c r="B450" s="4">
+        <v>45470</v>
+      </c>
+      <c r="C450" s="7">
+        <v>4</v>
+      </c>
+      <c r="D450" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E450" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F450" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G450" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H450" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I450" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="451" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A451" s="5">
+        <v>91338</v>
+      </c>
+      <c r="B451" s="4">
+        <v>45470</v>
+      </c>
+      <c r="C451" s="7">
+        <v>4</v>
+      </c>
+      <c r="D451" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E451" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F451" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G451" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H451" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J451" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="452" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A452" s="5">
+        <v>91339</v>
+      </c>
+      <c r="B452" s="4">
+        <v>45470</v>
+      </c>
+      <c r="C452" s="7">
+        <v>4</v>
+      </c>
+      <c r="D452" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E452" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F452" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G452" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H452" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I452" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="453" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A453" s="5">
+        <v>91339</v>
+      </c>
+      <c r="B453" s="4">
+        <v>45470</v>
+      </c>
+      <c r="C453" s="7">
+        <v>4</v>
+      </c>
+      <c r="D453" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E453" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F453" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G453" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H453" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J453" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="454" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A454" s="5">
+        <v>91340</v>
+      </c>
+      <c r="B454" s="4">
+        <v>45471</v>
+      </c>
+      <c r="C454" s="7">
+        <v>4</v>
+      </c>
+      <c r="D454" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E454" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F454" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G454" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H454" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I454" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="455" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A455" s="5">
+        <v>91340</v>
+      </c>
+      <c r="B455" s="4">
+        <v>45471</v>
+      </c>
+      <c r="C455" s="7">
+        <v>4</v>
+      </c>
+      <c r="D455" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E455" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F455" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G455" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H455" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J455" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="456" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A456" s="5">
+        <f>A454+1</f>
+        <v>91341</v>
+      </c>
+      <c r="B456" s="4">
+        <v>45471</v>
+      </c>
+      <c r="C456" s="7">
+        <v>4</v>
+      </c>
+      <c r="D456" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E456" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F456" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G456" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H456" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I456" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="457" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A457" s="5">
+        <f t="shared" ref="A457:A473" si="0">A455+1</f>
+        <v>91341</v>
+      </c>
+      <c r="B457" s="4">
+        <v>45471</v>
+      </c>
+      <c r="C457" s="7">
+        <v>4</v>
+      </c>
+      <c r="D457" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E457" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F457" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G457" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H457" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J457" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="458" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A458" s="5">
+        <f t="shared" si="0"/>
+        <v>91342</v>
+      </c>
+      <c r="B458" s="4">
+        <v>45471</v>
+      </c>
+      <c r="C458" s="7">
+        <v>4</v>
+      </c>
+      <c r="D458" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E458" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F458" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G458" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H458" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I458" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="459" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A459" s="5">
+        <f t="shared" si="0"/>
+        <v>91342</v>
+      </c>
+      <c r="B459" s="4">
+        <v>45471</v>
+      </c>
+      <c r="C459" s="7">
+        <v>4</v>
+      </c>
+      <c r="D459" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E459" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F459" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G459" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H459" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J459" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="460" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A460" s="5">
+        <f t="shared" si="0"/>
+        <v>91343</v>
+      </c>
+      <c r="B460" s="4">
+        <v>45471</v>
+      </c>
+      <c r="C460" s="7">
+        <v>4</v>
+      </c>
+      <c r="D460" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E460" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F460" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G460" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H460" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I460" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="461" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A461" s="5">
+        <f t="shared" si="0"/>
+        <v>91343</v>
+      </c>
+      <c r="B461" s="4">
+        <v>45471</v>
+      </c>
+      <c r="C461" s="7">
+        <v>4</v>
+      </c>
+      <c r="D461" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E461" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F461" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G461" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H461" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J461" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="462" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A462" s="5">
+        <f t="shared" si="0"/>
+        <v>91344</v>
+      </c>
+      <c r="B462" s="4">
+        <v>45471</v>
+      </c>
+      <c r="C462" s="7">
+        <v>4</v>
+      </c>
+      <c r="D462" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E462" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F462" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G462" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H462" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I462" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="463" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A463" s="5">
+        <f t="shared" si="0"/>
+        <v>91344</v>
+      </c>
+      <c r="B463" s="4">
+        <v>45471</v>
+      </c>
+      <c r="C463" s="7">
+        <v>4</v>
+      </c>
+      <c r="D463" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E463" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F463" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G463" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H463" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J463" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="464" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A464" s="5">
+        <f t="shared" si="0"/>
+        <v>91345</v>
+      </c>
+      <c r="B464" s="4">
+        <v>45472</v>
+      </c>
+      <c r="C464" s="7">
+        <v>4</v>
+      </c>
+      <c r="D464" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E464" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F464" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G464" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H464" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I464" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="465" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A465" s="5">
+        <f t="shared" si="0"/>
+        <v>91345</v>
+      </c>
+      <c r="B465" s="4">
+        <v>45472</v>
+      </c>
+      <c r="C465" s="7">
+        <v>4</v>
+      </c>
+      <c r="D465" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E465" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F465" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G465" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H465" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J465" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="466" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A466" s="5">
+        <f t="shared" si="0"/>
+        <v>91346</v>
+      </c>
+      <c r="B466" s="4">
+        <v>45472</v>
+      </c>
+      <c r="C466" s="7">
+        <v>4</v>
+      </c>
+      <c r="D466" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E466" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F466" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G466" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H466" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I466" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="467" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A467" s="5">
+        <f t="shared" si="0"/>
+        <v>91346</v>
+      </c>
+      <c r="B467" s="4">
+        <v>45472</v>
+      </c>
+      <c r="C467" s="7">
+        <v>4</v>
+      </c>
+      <c r="D467" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E467" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F467" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G467" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H467" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J467" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="468" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A468" s="5">
+        <f t="shared" si="0"/>
+        <v>91347</v>
+      </c>
+      <c r="B468" s="4">
+        <v>45472</v>
+      </c>
+      <c r="C468" s="7">
+        <v>4</v>
+      </c>
+      <c r="D468" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E468" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F468" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G468" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H468" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I468" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="469" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A469" s="5">
+        <f t="shared" si="0"/>
+        <v>91347</v>
+      </c>
+      <c r="B469" s="4">
+        <v>45472</v>
+      </c>
+      <c r="C469" s="7">
+        <v>4</v>
+      </c>
+      <c r="D469" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E469" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F469" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G469" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H469" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J469" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="470" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A470" s="5">
+        <f t="shared" si="0"/>
+        <v>91348</v>
+      </c>
+      <c r="B470" s="4">
+        <v>45472</v>
+      </c>
+      <c r="C470" s="7">
+        <v>4</v>
+      </c>
+      <c r="D470" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E470" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F470" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G470" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H470" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I470" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="471" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A471" s="5">
+        <f t="shared" si="0"/>
+        <v>91348</v>
+      </c>
+      <c r="B471" s="4">
+        <v>45472</v>
+      </c>
+      <c r="C471" s="7">
+        <v>4</v>
+      </c>
+      <c r="D471" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E471" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F471" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G471" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H471" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J471" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="472" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A472" s="5">
+        <f t="shared" si="0"/>
+        <v>91349</v>
+      </c>
+      <c r="B472" s="4">
+        <v>45472</v>
+      </c>
+      <c r="C472" s="7">
+        <v>4</v>
+      </c>
+      <c r="D472" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E472" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F472" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G472" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H472" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I472" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="473" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A473" s="5">
+        <f t="shared" si="0"/>
+        <v>91349</v>
+      </c>
+      <c r="B473" s="4">
+        <v>45472</v>
+      </c>
+      <c r="C473" s="7">
+        <v>4</v>
+      </c>
+      <c r="D473" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E473" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F473" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G473" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H473" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J473" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
last update before Champs!!
</commit_message>
<xml_diff>
--- a/v04/data/vetoes.xlsx
+++ b/v04/data/vetoes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a37d342720a2caaa/Desktop/dataClass/06-cod-analysis/03 CDL PrizePicks Betting/cdl_prizepicks_betting_apps/v04/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3289" documentId="11_05A95047836714DFE54878D6425DCE3A87460B4D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E6D0AD2-C40C-403F-BEF4-2DD827C506D3}"/>
+  <xr:revisionPtr revIDLastSave="3356" documentId="11_05A95047836714DFE54878D6425DCE3A87460B4D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8CE11D1-D752-4DBF-9D75-B05330F79674}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9525" yWindow="0" windowWidth="9750" windowHeight="10155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2842" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2890" uniqueCount="32">
   <si>
     <t>match_id</t>
   </si>
@@ -510,11 +510,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J473"/>
+  <dimension ref="A1:J481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A455" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K471" sqref="K471"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A461" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J482" sqref="J482"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -13756,7 +13756,7 @@
     </row>
     <row r="457" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A457" s="5">
-        <f t="shared" ref="A457:A473" si="0">A455+1</f>
+        <f t="shared" ref="A457:A481" si="0">A455+1</f>
         <v>91341</v>
       </c>
       <c r="B457" s="4">
@@ -14264,6 +14264,246 @@
         <v>21</v>
       </c>
     </row>
+    <row r="474" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A474" s="5">
+        <f t="shared" si="0"/>
+        <v>91350</v>
+      </c>
+      <c r="B474" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C474" s="7">
+        <v>4</v>
+      </c>
+      <c r="D474" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E474" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F474" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G474" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H474" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I474" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="475" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A475" s="5">
+        <f t="shared" si="0"/>
+        <v>91350</v>
+      </c>
+      <c r="B475" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C475" s="7">
+        <v>4</v>
+      </c>
+      <c r="D475" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E475" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F475" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G475" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H475" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J475" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="476" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A476" s="5">
+        <f t="shared" si="0"/>
+        <v>91351</v>
+      </c>
+      <c r="B476" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C476" s="7">
+        <v>4</v>
+      </c>
+      <c r="D476" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E476" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F476" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G476" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H476" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I476" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="477" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A477" s="5">
+        <f t="shared" si="0"/>
+        <v>91351</v>
+      </c>
+      <c r="B477" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C477" s="7">
+        <v>4</v>
+      </c>
+      <c r="D477" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E477" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F477" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G477" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H477" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J477" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="478" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A478" s="5">
+        <f t="shared" si="0"/>
+        <v>91352</v>
+      </c>
+      <c r="B478" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C478" s="7">
+        <v>4</v>
+      </c>
+      <c r="D478" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E478" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F478" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G478" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H478" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I478" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="479" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A479" s="5">
+        <f t="shared" si="0"/>
+        <v>91352</v>
+      </c>
+      <c r="B479" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C479" s="7">
+        <v>4</v>
+      </c>
+      <c r="D479" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E479" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F479" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G479" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H479" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J479" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="480" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A480" s="5">
+        <f t="shared" si="0"/>
+        <v>91353</v>
+      </c>
+      <c r="B480" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C480" s="7">
+        <v>4</v>
+      </c>
+      <c r="D480" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E480" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F480" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G480" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H480" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I480" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="481" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A481" s="5">
+        <f t="shared" si="0"/>
+        <v>91353</v>
+      </c>
+      <c r="B481" s="4">
+        <v>45473</v>
+      </c>
+      <c r="C481" s="7">
+        <v>4</v>
+      </c>
+      <c r="D481" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E481" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F481" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G481" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H481" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J481" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>